<commit_message>
Commit the latest code
</commit_message>
<xml_diff>
--- a/MavenDemSelArtifact/dataDemo.xlsx
+++ b/MavenDemSelArtifact/dataDemo.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.b.ramamurthy\Docsis\SelTraining\src\test\java\demoDataDrivenTesting\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD5F30-5488-4C8E-979C-4C3035713069}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1E4D6A3B-BB2A-4313-9681-80C237A22372}"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="6615"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -75,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -236,7 +231,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -430,24 +425,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233C8A80-EF87-404B-9D8E-ABF34159A614}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -501,13 +496,13 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{3F754C26-62B5-48CD-8B2D-D06713432DD8}"/>
-    <hyperlink ref="A2:A6" r:id="rId2" display="username1@xyz.com" xr:uid="{4C31000D-BF53-4BDC-A1FD-F3EF671B5AB1}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{FA21AA97-0CF9-4E4F-8551-6BEBBB378BE0}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{D02C58D9-552C-4FCE-9183-BAC7528913D9}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{582035A4-8A49-49B3-88A3-12D409146EA3}"/>
-    <hyperlink ref="A5" r:id="rId6" xr:uid="{A40305F9-D3BC-4100-AE20-49BCFE5DD354}"/>
-    <hyperlink ref="A6" r:id="rId7" xr:uid="{E618533B-E889-4193-A8DF-BE61E52AE646}"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2:A6" r:id="rId2" display="username1@xyz.com"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="A5" r:id="rId6"/>
+    <hyperlink ref="A6" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>